<commit_message>
âœ¨ Ajout de la lemmatisation avec spaCy - Analyse linguistique professionnelle
- IntÃ©gration de spaCy fr_core_news_sm pour lemmatisation avancÃ©e
- RÃ©duction de ~50% du volume de mots avec prÃ©cision linguistique
- Mise Ã  jour de tous les rÃ©sultats avec les lemmes
- Documentation complÃ¨te de la technique (LEMMATISATION_EXPLICATIONS.md)
- Mise Ã  jour README et TECHNIQUES_TEXT_MINING.md
- requirements.txt mis Ã  jour avec spaCy

Impact :
- PAM: 1067 â†’ 535 lemmes (50%)
- PI: 5370 â†’ 2492 lemmes (54%)
- PJD: 1605 â†’ 746 lemmes (54%)
- RNI: 1688 â†’ 858 lemmes (49%)
</commit_message>
<xml_diff>
--- a/cooccurrences_themes.xlsx
+++ b/cooccurrences_themes.xlsx
@@ -468,11 +468,11 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Social</t>
+          <t>Environnement</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3">
@@ -483,16 +483,16 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Gouvernance</t>
+          <t>Emploi</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Social</t>
+          <t>Justice</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4">
@@ -512,7 +512,7 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5">
@@ -528,11 +528,11 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Santé</t>
+          <t>Économie</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6">
@@ -543,7 +543,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Emploi</t>
+          <t>Gouvernance</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -552,7 +552,7 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7">
@@ -563,7 +563,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Santé</t>
+          <t>Emploi</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -572,7 +572,7 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8">
@@ -583,16 +583,16 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Emploi</t>
+          <t>Environnement</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Économie</t>
+          <t>Gouvernance</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9">
@@ -603,16 +603,16 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Gouvernance</t>
+          <t>Emploi</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Économie</t>
+          <t>Santé</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10">
@@ -623,7 +623,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Social</t>
+          <t>Environnement</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -632,7 +632,7 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11">
@@ -643,16 +643,16 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Justice</t>
+          <t>Gouvernance</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Social</t>
+          <t>Économie</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12">
@@ -672,7 +672,7 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>67</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13">
@@ -683,7 +683,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Social</t>
+          <t>Gouvernance</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -692,7 +692,7 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>51</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14">
@@ -703,16 +703,16 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Environnement</t>
+          <t>Justice</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Social</t>
+          <t>Économie</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>50</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15">
@@ -723,16 +723,16 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Gouvernance</t>
+          <t>Environnement</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Économie</t>
+          <t>Gouvernance</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>43</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16">
@@ -743,16 +743,16 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Environnement</t>
+          <t>Social</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Gouvernance</t>
+          <t>Économie</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>39</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17">
@@ -763,16 +763,16 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Agriculture</t>
+          <t>Environnement</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Environnement</t>
+          <t>Justice</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>37</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18">
@@ -783,16 +783,16 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Agriculture</t>
+          <t>Gouvernance</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Économie</t>
+          <t>Social</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19">
@@ -803,7 +803,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Gouvernance</t>
+          <t>Justice</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -812,7 +812,7 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>33</v>
+        <v>25</v>
       </c>
     </row>
     <row r="20">
@@ -823,16 +823,16 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Justice</t>
+          <t>Gouvernance</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Économie</t>
+          <t>Justice</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>33</v>
+        <v>24</v>
       </c>
     </row>
     <row r="21">
@@ -843,16 +843,16 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Environnement</t>
+          <t>Infrastructure</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Justice</t>
+          <t>Économie</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>32</v>
+        <v>23</v>
       </c>
     </row>
     <row r="22">
@@ -863,16 +863,16 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Gouvernance</t>
+          <t>Environnement</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Social</t>
+          <t>Gouvernance</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="23">
@@ -883,16 +883,16 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Environnement</t>
+          <t>Gouvernance</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Gouvernance</t>
+          <t>Justice</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24">
@@ -908,11 +908,11 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Justice</t>
+          <t>Social</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="25">
@@ -923,16 +923,16 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Justice</t>
+          <t>Environnement</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Social</t>
+          <t>Justice</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="26">
@@ -943,16 +943,16 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Gouvernance</t>
+          <t>Justice</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Économie</t>
+          <t>Social</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="27">
@@ -963,16 +963,16 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Justice</t>
+          <t>Environnement</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Économie</t>
+          <t>Social</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="28">
@@ -992,7 +992,7 @@
         </is>
       </c>
       <c r="D28" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="29">
@@ -1003,12 +1003,12 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Emploi</t>
+          <t>Gouvernance</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Jeunesse</t>
+          <t>Économie</t>
         </is>
       </c>
       <c r="D29" t="n">
@@ -1023,16 +1023,16 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Environnement</t>
+          <t>Justice</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Justice</t>
+          <t>Économie</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="31">
@@ -1052,7 +1052,7 @@
         </is>
       </c>
       <c r="D31" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="32">
@@ -1072,7 +1072,7 @@
         </is>
       </c>
       <c r="D32" t="n">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="33">
@@ -1092,7 +1092,7 @@
         </is>
       </c>
       <c r="D33" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="34">
@@ -1112,7 +1112,7 @@
         </is>
       </c>
       <c r="D34" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="35">
@@ -1123,7 +1123,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Emploi</t>
+          <t>Social</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1148,11 +1148,11 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Santé</t>
+          <t>Économie</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="37">
@@ -1163,12 +1163,12 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Justice</t>
+          <t>Gouvernance</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Économie</t>
+          <t>Justice</t>
         </is>
       </c>
       <c r="D37" t="n">
@@ -1183,7 +1183,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Social</t>
+          <t>Justice</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -1203,16 +1203,16 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Justice</t>
+          <t>Emploi</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Santé</t>
+          <t>Gouvernance</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="40">
@@ -1223,12 +1223,12 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Emploi</t>
+          <t>Droits_Femme</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Gouvernance</t>
+          <t>Social</t>
         </is>
       </c>
       <c r="D40" t="n">
@@ -1248,11 +1248,11 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Justice</t>
+          <t>Social</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>